<commit_message>
chore: added test functionality
</commit_message>
<xml_diff>
--- a/validation_tests/inputs/test_data_model/devices.xlsx
+++ b/validation_tests/inputs/test_data_model/devices.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\fiware-api-tests\validation_tests\inputs\test_data_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sba\PycharmProjects\fiware-api-tests\validation_tests\inputs\test_data_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17565179-1C1E-406C-B5E5-6C850C599D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42132" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42130" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -67,15 +66,12 @@
   </si>
   <si>
     <t>Adeunis modbus</t>
-  </si>
-  <si>
-    <t>eui-0018b2400001a3fd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,7 +106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -387,22 +383,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.453125" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,7 +406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -419,7 +415,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -428,7 +424,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -437,7 +433,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -446,7 +442,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -455,7 +451,7 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -464,7 +460,7 @@
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -473,7 +469,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -482,7 +478,7 @@
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -492,74 +488,56 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>

</xml_diff>